<commit_message>
Atualização automática de tabela concluida
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">img_back</t>
   </si>
   <si>
-    <t xml:space="preserve">highlighs</t>
+    <t xml:space="preserve">highlights</t>
   </si>
   <si>
     <t xml:space="preserve">is_available</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">camisa azul</t>
+    <t xml:space="preserve">camisa laranja</t>
   </si>
   <si>
     <t xml:space="preserve">299.99</t>
@@ -100,19 +100,19 @@
     <t xml:space="preserve">true</t>
   </si>
   <si>
-    <t xml:space="preserve">camisa vermelha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">199.99</t>
+    <t xml:space="preserve">camisa pessego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">899.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.99</t>
   </si>
   <si>
     <t xml:space="preserve">SKU-245345</t>
   </si>
   <si>
-    <t xml:space="preserve">Camisa-vermelha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
+    <t xml:space="preserve">Camisa-rosa</t>
   </si>
 </sst>
 </file>
@@ -122,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -143,6 +143,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -193,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,6 +210,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,11 +236,11 @@
   </sheetPr>
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.41"/>
@@ -240,7 +251,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="32.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,8 +297,8 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -347,13 +358,13 @@
         <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>20</v>
@@ -371,7 +382,7 @@
         <v>24</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Corrigindo erros de 'id' duplicado
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">camisa laranja</t>
+    <t xml:space="preserve">Camisa 233323</t>
   </si>
   <si>
     <t xml:space="preserve">299.99</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">399.99</t>
   </si>
   <si>
-    <t xml:space="preserve">SKU-2872163</t>
+    <t xml:space="preserve">SKU-hdhdhdhdh</t>
   </si>
   <si>
     <t xml:space="preserve">Camisa-azul</t>
@@ -97,22 +97,88 @@
     <t xml:space="preserve">https://i.imgur.com/hTBFx7g.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">camisa aslkdla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">899.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU-245345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camisa-rosa</t>
+  </si>
+  <si>
     <t xml:space="preserve">true</t>
   </si>
   <si>
-    <t xml:space="preserve">camisa pessego</t>
-  </si>
-  <si>
-    <t xml:space="preserve">899.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">99.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKU-245345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camisa-rosa</t>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">camisa emily2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camisa-preta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccassmdiasmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfsdfsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsdfsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfsdfsdfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfsdfsdfsdfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfsdfsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sadasdsdfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghfghfgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghfghfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghfghfghfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghfghfghfgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fghfghfghfghfghfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfghfghfghfg</t>
   </si>
 </sst>
 </file>
@@ -234,13 +300,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.41"/>
@@ -382,9 +448,185 @@
         <v>24</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>34534</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>45345</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>456456</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>5645</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>7869789</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>67867</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="0" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>